<commit_message>
minor cleanups, move to sets as flow.
</commit_message>
<xml_diff>
--- a/AudioVideo_Fields.xlsx
+++ b/AudioVideo_Fields.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="140">
   <si>
     <t xml:space="preserve">audiocassette</t>
   </si>
@@ -361,7 +361,10 @@
   </si>
   <si>
     <t xml:space="preserve">Tape speed in ips.  
-Single or set of Values: 15, 7.5, 3.75, 1.875.  </t>
+Set of Values: 15, 7.5, 3.75, 1.875.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[7.5]</t>
   </si>
   <si>
     <t xml:space="preserve">noise_reduction</t>
@@ -457,6 +460,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -516,28 +520,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -666,929 +678,929 @@
   </sheetPr>
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="0" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="Q38" activeCellId="0" sqref="Q38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="0" topLeftCell="F13" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topRight" activeCell="K32" activeCellId="0" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="29.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="29.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="26.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="25.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="4.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="29.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="29.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="26.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="25.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="12.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="O4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="Q4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="F10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K10" s="3" t="s">
+      <c r="I10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="L10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N10" s="0" t="s">
+      <c r="L10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q10" s="0" t="s">
+      <c r="O10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="3" t="s">
+      <c r="F11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" s="3" t="s">
+      <c r="I11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="K11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M11" s="0" t="s">
+      <c r="L11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="N11" s="0" t="s">
+      <c r="N11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="O11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P11" s="0" t="s">
+      <c r="O11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Q11" s="0" t="s">
+      <c r="Q11" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="3" t="s">
+      <c r="F12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" s="3" t="s">
+      <c r="I12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K12" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N12" s="0" t="s">
+      <c r="L12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="O12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P12" s="0" t="s">
+      <c r="O12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Q12" s="0" t="s">
+      <c r="Q12" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="J13" s="0" t="n">
+      <c r="J13" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="K13" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="M13" s="0" t="s">
+      <c r="M13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="N13" s="0" t="s">
+      <c r="N13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="O13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="P13" s="0" t="s">
+      <c r="P13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Q13" s="0" t="s">
+      <c r="Q13" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L14" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="M14" s="0" t="s">
+      <c r="M14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="N14" s="0" t="s">
+      <c r="N14" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="J15" s="0" t="n">
+      <c r="J15" s="1" t="n">
         <v>1.4</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="K15" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="K17" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="J18" s="0" t="n">
+      <c r="J18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K18" s="0" t="n">
+      <c r="K18" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="J19" s="0" t="n">
+      <c r="J19" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="I23" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="J23" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="K23" s="4" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="I24" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="J24" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="K24" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="L24" s="2" t="s">
+      <c r="L24" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="M24" s="0" t="s">
+      <c r="M24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N24" s="0" t="s">
+      <c r="N24" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O24" s="2" t="s">
+      <c r="O24" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="P24" s="0" t="s">
+      <c r="P24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="Q24" s="0" t="s">
+      <c r="Q24" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="L25" s="2" t="s">
+      <c r="L25" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="M25" s="4" t="n">
+      <c r="M25" s="6" t="n">
         <v>45374</v>
       </c>
-      <c r="N25" s="3" t="s">
+      <c r="N25" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="O25" s="2" t="s">
+      <c r="O25" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="P25" s="4" t="n">
+      <c r="P25" s="6" t="n">
         <v>45374</v>
       </c>
-      <c r="Q25" s="3" t="s">
+      <c r="Q25" s="4" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="L26" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="M26" s="3" t="s">
+      <c r="M26" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="N26" s="3" t="s">
+      <c r="N26" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="O26" s="2" t="s">
+      <c r="O26" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="P26" s="3" t="s">
+      <c r="P26" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="Q26" s="3" t="s">
+      <c r="Q26" s="4" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H29" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J29" s="3" t="s">
+      <c r="I29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J29" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="K29" s="3" t="s">
+      <c r="K29" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="L29" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M29" s="3" t="s">
+      <c r="L29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M29" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="N29" s="3" t="s">
+      <c r="N29" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="O29" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P29" s="3" t="s">
+      <c r="O29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P29" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="Q29" s="3" t="s">
+      <c r="Q29" s="4" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="0" t="s">
+      <c r="E30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="H30" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I30" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K30" s="3" t="s">
+      <c r="I30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="L30" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N30" s="3" t="s">
+      <c r="L30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N30" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="O30" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q30" s="3" t="s">
+      <c r="O30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q30" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-    </row>
-    <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+    </row>
+    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="E32" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="H32" s="0" t="n">
+      <c r="H32" s="1" t="n">
         <v>1.875</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="I32" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="K32" s="0" t="n">
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
+      <c r="K32" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C33" s="0" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="C33" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G33" s="3" t="s">
+      <c r="F33" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="G33" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="H33" s="4" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="C34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="C34" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G34" s="3" t="s">
+      <c r="F34" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="H34" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="I34" s="2" t="s">
+      <c r="G34" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="J34" s="3" t="s">
+      <c r="H34" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I34" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="K34" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="L34" s="2" t="s">
+      <c r="J34" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="M34" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="N34" s="3" t="s">
+      <c r="K34" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="N34" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="O34" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="P34" s="3" t="s">
+      <c r="O34" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="Q34" s="3" t="s">
+      <c r="P34" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q34" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="C35" s="0" t="s">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="C35" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="L35" s="2" t="s">
+      <c r="E35" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="M35" s="3" t="s">
+      <c r="L35" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="N35" s="3" t="s">
+      <c r="M35" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="O35" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="O35" s="2" t="s">
+      <c r="P35" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q35" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="P35" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q35" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="M36" s="5" t="s">
+      <c r="L36" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="N36" s="5" t="s">
+      <c r="M36" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="O36" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="P36" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q36" s="5" t="s">
-        <v>134</v>
+      <c r="N36" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="O36" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="P36" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q36" s="7" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="L37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="O37" s="2" t="s">
+      <c r="L37" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="P37" s="3" t="s">
+      <c r="O37" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="Q37" s="3" t="s">
-        <v>138</v>
+      <c r="P37" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q37" s="4" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>